<commit_message>
Ikke generer  Excelfil i svar
</commit_message>
<xml_diff>
--- a/src/main/resources/bulk-upload/koronasykepengerefusjon_nav.xlsx
+++ b/src/main/resources/bulk-upload/koronasykepengerefusjon_nav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommy/Dropbox/NAV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B152317\J SPORENSTREKS\Info LPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75EED203-6199-434C-AE3F-06F484D8D6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89159AE3-7EEA-46A5-A2F7-32FACEFE81E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D6DC71BC-B5E6-104F-ACAE-6ED12C21E25B}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" xr2:uid="{D6DC71BC-B5E6-104F-ACAE-6ED12C21E25B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>3514</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Fødselsnummer</t>
-  </si>
-  <si>
-    <t>Organisasjonsnummer</t>
   </si>
   <si>
     <t>Fra og med</t>
@@ -60,8 +57,26 @@
     <t>12345678901</t>
   </si>
   <si>
+    <t>15.03.2020</t>
+  </si>
+  <si>
+    <t>Slik fylles tallene inn:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begynn å fylle ut på rad 11 </t>
+  </si>
+  <si>
+    <t>Virksomhetsnummer</t>
+  </si>
+  <si>
+    <t>Antall arbeidsdager som kreves refundert</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Dette dokumentet er beregnet på bedrifter som har for mange ansatte til at et vanlig web-skjema er praktisk. </t>
+      <t xml:space="preserve">Dette dokumentet er beregnet på virksomheter som har for mange ansatte til at et vanlig web-skjema er praktisk. </t>
     </r>
     <r>
       <rPr>
@@ -72,7 +87,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Du kan max legge til 5000 ansatte.</t>
+      <t>Du kan max legge til 5000 arbeidstakere.</t>
     </r>
     <r>
       <rPr>
@@ -82,20 +97,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Er ikke dette tilstrekkelig må du fylle ut og laste opp i flere omganger. </t>
+      <t xml:space="preserve"> Er ikke dette tilstrekkelig, må du fylle ut og laste opp i flere omganger. </t>
     </r>
   </si>
   <si>
-    <t>15.03.2020</t>
+    <t>123456789</t>
   </si>
   <si>
-    <t>Fraværsperiode (DD.MM.ÅÅÅÅ)</t>
-  </si>
-  <si>
-    <t>Slik fylles tallene inn:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Begynn å fylle ut på rad 11 </t>
+    <t>Fraværsperiode (DD.MM.YYYY)</t>
   </si>
 </sst>
 </file>
@@ -538,21 +547,22 @@
   <dimension ref="A1:Q2874"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" style="6" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="39.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.59765625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="37">
+    <row r="1" spans="1:17" ht="34.799999999999997">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -576,7 +586,7 @@
     </row>
     <row r="4" spans="1:17" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="1"/>
@@ -597,7 +607,7 @@
     </row>
     <row r="5" spans="1:17" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
@@ -618,21 +628,23 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
-        <v>123456785</v>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -651,7 +663,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -666,36 +678,41 @@
     </row>
     <row r="8" spans="1:17" s="10" customFormat="1" ht="21">
       <c r="A8" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:17" s="10" customFormat="1">
       <c r="A9" s="1"/>
       <c r="B9" s="7"/>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:17" s="14" customFormat="1" ht="21">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>5</v>
+      <c r="E10" s="13" t="s">
+        <v>12</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>1</v>
       </c>
     </row>
@@ -9293,5 +9310,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>